<commit_message>
Add new bill management functionality with data visualization in bill.py; update event handling in functions.py; add weather reporting capabilities in whether.py; and include necessary build files for packaging.
</commit_message>
<xml_diff>
--- a/files/schedule.xlsx
+++ b/files/schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
   <si>
     <t>time</t>
   </si>
@@ -46,18 +46,24 @@
     <t>吃饭</t>
   </si>
   <si>
+    <t>晨跑</t>
+  </si>
+  <si>
     <t>8:50-9:30</t>
   </si>
   <si>
     <t>9:30-10:00</t>
   </si>
   <si>
-    <t>哈哈哈哈</t>
+    <t>写作业预习</t>
   </si>
   <si>
     <t>10:00-10:40</t>
   </si>
   <si>
+    <t>上课</t>
+  </si>
+  <si>
     <t>吃吃饭</t>
   </si>
   <si>
@@ -70,16 +76,19 @@
     <t>13:00-13:30</t>
   </si>
   <si>
-    <t>go to the shopping mall</t>
-  </si>
-  <si>
-    <t>17:00-23:30</t>
+    <t>14:00-14:30</t>
   </si>
   <si>
     <t>15:00-15:30</t>
   </si>
   <si>
+    <t>和女朋友见面</t>
+  </si>
+  <si>
     <t>16:00-16:30</t>
+  </si>
+  <si>
+    <t>健身</t>
   </si>
   <si>
     <t>17:00-17:30</t>
@@ -90,10 +99,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -107,6 +116,20 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,35 +143,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -157,68 +151,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,9 +174,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,31 +266,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,151 +440,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,26 +469,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,8 +502,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,16 +535,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,142 +562,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1027,7 +1036,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D12" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -1070,10 +1079,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1087,15 +1096,11 @@
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3"/>
       <c r="E3" t="s">
         <v>9</v>
       </c>
@@ -1111,16 +1116,16 @@
     </row>
     <row r="4" ht="44" customHeight="1" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -1137,22 +1142,22 @@
     </row>
     <row r="5" ht="44" customHeight="1" spans="1:8">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -1163,22 +1168,22 @@
     </row>
     <row r="6" ht="44" customHeight="1" spans="1:8">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -1189,7 +1194,7 @@
     </row>
     <row r="7" ht="44" customHeight="1" spans="1:8">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -1198,7 +1203,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -1215,16 +1220,16 @@
     </row>
     <row r="8" ht="44" customHeight="1" spans="1:8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -1241,16 +1246,16 @@
     </row>
     <row r="9" ht="44" customHeight="1" spans="1:8">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -1267,16 +1272,16 @@
     </row>
     <row r="10" ht="44" customHeight="1" spans="1:8">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1293,7 +1298,7 @@
     </row>
     <row r="11" ht="44" customHeight="1" spans="1:8">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>

</xml_diff>